<commit_message>
Update archive for manually reconciled entries
</commit_message>
<xml_diff>
--- a/ArchiveForReconciledEntries/MusicBrainz_archiveForManuallyReconciledEntries.xlsx
+++ b/ArchiveForReconciledEntries/MusicBrainz_archiveForManuallyReconciledEntries.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28440" windowHeight="13040" activeTab="7"/>
+    <workbookView windowHeight="12500" tabRatio="760" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="area_type" sheetId="1" r:id="rId1"/>
@@ -2922,7 +2922,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2930,9 +2930,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1">
@@ -3505,15 +3502,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
@@ -3521,7 +3518,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
@@ -3529,7 +3526,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
@@ -3537,7 +3534,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
@@ -3545,12 +3542,12 @@
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
@@ -3558,7 +3555,7 @@
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B8" t="s">
@@ -3566,7 +3563,7 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B9" t="s">
@@ -3574,7 +3571,7 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B10" t="s">
@@ -3582,8 +3579,8 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3606,23 +3603,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" ht="18" spans="1:2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" ht="18" spans="1:2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -3630,7 +3627,7 @@
       </c>
     </row>
     <row r="4" ht="18" spans="1:2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -3638,7 +3635,7 @@
       </c>
     </row>
     <row r="5" ht="18" spans="1:2">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -3646,12 +3643,12 @@
       </c>
     </row>
     <row r="6" ht="18" spans="1:1">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" ht="18" spans="1:2">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -3686,10 +3683,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -3705,7 +3702,7 @@
       <c r="A3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3713,7 +3710,7 @@
       <c r="A4" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3721,7 +3718,7 @@
       <c r="A5" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3777,10 +3774,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -3788,7 +3785,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B2" t="s">
@@ -3796,7 +3793,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B3" t="s">
@@ -3804,7 +3801,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B4" t="s">
@@ -3812,7 +3809,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>51</v>
       </c>
       <c r="B5" t="s">
@@ -3820,7 +3817,7 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>53</v>
       </c>
       <c r="B6" t="s">
@@ -3828,7 +3825,7 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>55</v>
       </c>
       <c r="B7" t="s">
@@ -3839,7 +3836,7 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>58</v>
       </c>
       <c r="B8" t="s">
@@ -3850,7 +3847,7 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>60</v>
       </c>
       <c r="B9" t="s">
@@ -3858,7 +3855,7 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>62</v>
       </c>
       <c r="B10" t="s">
@@ -3866,7 +3863,7 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>64</v>
       </c>
       <c r="B11" t="s">
@@ -3902,19 +3899,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="3"/>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
@@ -4193,9 +4190,9 @@
       <c r="C26" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
@@ -4207,9 +4204,9 @@
       <c r="C27" t="s">
         <v>145</v>
       </c>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
@@ -4221,9 +4218,9 @@
       <c r="C28" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
@@ -4235,9 +4232,9 @@
       <c r="C29" t="s">
         <v>151</v>
       </c>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
@@ -4249,9 +4246,9 @@
       <c r="C30" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
@@ -4263,9 +4260,9 @@
       <c r="C31" t="s">
         <v>157</v>
       </c>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
@@ -4277,9 +4274,9 @@
       <c r="C32" t="s">
         <v>160</v>
       </c>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
@@ -4291,9 +4288,9 @@
       <c r="C33" t="s">
         <v>163</v>
       </c>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
@@ -4305,9 +4302,9 @@
       <c r="C34" t="s">
         <v>166</v>
       </c>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
@@ -4319,9 +4316,9 @@
       <c r="C35" t="s">
         <v>169</v>
       </c>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
@@ -4333,9 +4330,9 @@
       <c r="C36" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
@@ -4347,9 +4344,9 @@
       <c r="C37" t="s">
         <v>175</v>
       </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
@@ -4361,9 +4358,9 @@
       <c r="C38" t="s">
         <v>178</v>
       </c>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
@@ -4375,9 +4372,9 @@
       <c r="C39" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
@@ -4389,9 +4386,9 @@
       <c r="C40" t="s">
         <v>184</v>
       </c>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
@@ -4403,9 +4400,9 @@
       <c r="C41" t="s">
         <v>187</v>
       </c>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
@@ -4417,9 +4414,9 @@
       <c r="C42" t="s">
         <v>190</v>
       </c>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
@@ -4431,9 +4428,9 @@
       <c r="C43" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
@@ -4445,9 +4442,9 @@
       <c r="C44" t="s">
         <v>196</v>
       </c>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
@@ -4459,9 +4456,9 @@
       <c r="C45" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
@@ -4473,9 +4470,9 @@
       <c r="C46" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
@@ -4487,9 +4484,9 @@
       <c r="C47" t="s">
         <v>205</v>
       </c>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
@@ -4501,9 +4498,9 @@
       <c r="C48" t="s">
         <v>208</v>
       </c>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
@@ -4515,9 +4512,9 @@
       <c r="C49" t="s">
         <v>211</v>
       </c>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
@@ -4529,9 +4526,9 @@
       <c r="C50" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
@@ -4543,9 +4540,9 @@
       <c r="C51" t="s">
         <v>217</v>
       </c>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
@@ -4557,9 +4554,9 @@
       <c r="C52" t="s">
         <v>220</v>
       </c>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
@@ -4571,9 +4568,9 @@
       <c r="C53" t="s">
         <v>223</v>
       </c>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
@@ -4585,9 +4582,9 @@
       <c r="C54" t="s">
         <v>226</v>
       </c>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
@@ -4599,9 +4596,9 @@
       <c r="C55" t="s">
         <v>229</v>
       </c>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
@@ -4613,13 +4610,13 @@
       <c r="C56" t="s">
         <v>232</v>
       </c>
-      <c r="E56" s="5" t="s">
+      <c r="E56" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F56" s="5">
+      <c r="F56" s="4">
         <v>262</v>
       </c>
-      <c r="G56" s="5" t="s">
+      <c r="G56" s="4" t="s">
         <v>232</v>
       </c>
     </row>
@@ -4633,9 +4630,9 @@
       <c r="C57" t="s">
         <v>236</v>
       </c>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
-      <c r="G57" s="5"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
@@ -4647,13 +4644,13 @@
       <c r="C58" t="s">
         <v>239</v>
       </c>
-      <c r="E58" s="5" t="s">
+      <c r="E58" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F58" s="5">
+      <c r="F58" s="4">
         <v>191</v>
       </c>
-      <c r="G58" s="5" t="s">
+      <c r="G58" s="4" t="s">
         <v>239</v>
       </c>
     </row>
@@ -4667,9 +4664,9 @@
       <c r="C59" t="s">
         <v>242</v>
       </c>
-      <c r="E59" s="5"/>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
@@ -4681,9 +4678,9 @@
       <c r="C60" t="s">
         <v>245</v>
       </c>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
@@ -4695,9 +4692,9 @@
       <c r="C61" t="s">
         <v>248</v>
       </c>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
@@ -4709,9 +4706,9 @@
       <c r="C62" t="s">
         <v>251</v>
       </c>
-      <c r="E62" s="5"/>
-      <c r="F62" s="5"/>
-      <c r="G62" s="5"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
@@ -4723,9 +4720,9 @@
       <c r="C63" t="s">
         <v>254</v>
       </c>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
@@ -4737,9 +4734,9 @@
       <c r="C64" t="s">
         <v>257</v>
       </c>
-      <c r="E64" s="5"/>
-      <c r="F64" s="5"/>
-      <c r="G64" s="5"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
@@ -4751,9 +4748,9 @@
       <c r="C65" t="s">
         <v>260</v>
       </c>
-      <c r="E65" s="5"/>
-      <c r="F65" s="5"/>
-      <c r="G65" s="5"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
@@ -4765,13 +4762,13 @@
       <c r="C66" t="s">
         <v>263</v>
       </c>
-      <c r="E66" s="5" t="s">
+      <c r="E66" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F66" s="5">
+      <c r="F66" s="4">
         <v>145</v>
       </c>
-      <c r="G66" s="5" t="s">
+      <c r="G66" s="4" t="s">
         <v>263</v>
       </c>
     </row>
@@ -4785,9 +4782,9 @@
       <c r="C67" t="s">
         <v>266</v>
       </c>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="5"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" t="s">
@@ -4799,13 +4796,13 @@
       <c r="C68" t="s">
         <v>269</v>
       </c>
-      <c r="E68" s="5" t="s">
+      <c r="E68" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F68" s="5">
+      <c r="F68" s="4">
         <v>230</v>
       </c>
-      <c r="G68" s="5" t="s">
+      <c r="G68" s="4" t="s">
         <v>269</v>
       </c>
     </row>
@@ -4819,13 +4816,13 @@
       <c r="C69" t="s">
         <v>272</v>
       </c>
-      <c r="E69" s="5" t="s">
+      <c r="E69" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F69" s="5">
+      <c r="F69" s="4">
         <v>3769</v>
       </c>
-      <c r="G69" s="5" t="s">
+      <c r="G69" s="4" t="s">
         <v>272</v>
       </c>
     </row>
@@ -4839,13 +4836,13 @@
       <c r="C70" t="s">
         <v>275</v>
       </c>
-      <c r="E70" s="5" t="s">
+      <c r="E70" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F70" s="5">
+      <c r="F70" s="4">
         <v>25230</v>
       </c>
-      <c r="G70" s="5" t="s">
+      <c r="G70" s="4" t="s">
         <v>275</v>
       </c>
     </row>
@@ -4914,13 +4911,13 @@
       <c r="C76" t="s">
         <v>293</v>
       </c>
-      <c r="E76" s="5" t="s">
+      <c r="E76" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F76" s="5">
+      <c r="F76" s="4">
         <v>17012</v>
       </c>
-      <c r="G76" s="5" t="s">
+      <c r="G76" s="4" t="s">
         <v>293</v>
       </c>
     </row>
@@ -4934,9 +4931,9 @@
       <c r="C77" t="s">
         <v>296</v>
       </c>
-      <c r="E77" s="5"/>
-      <c r="F77" s="5"/>
-      <c r="G77" s="5"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
+      <c r="G77" s="4"/>
     </row>
     <row r="78" spans="1:7">
       <c r="A78" t="s">
@@ -4948,9 +4945,9 @@
       <c r="C78" t="s">
         <v>299</v>
       </c>
-      <c r="E78" s="5"/>
-      <c r="F78" s="5"/>
-      <c r="G78" s="5"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="4"/>
+      <c r="G78" s="4"/>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" t="s">
@@ -4962,13 +4959,13 @@
       <c r="C79" t="s">
         <v>302</v>
       </c>
-      <c r="E79" s="5" t="s">
+      <c r="E79" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F79" s="5">
+      <c r="F79" s="4">
         <v>774</v>
       </c>
-      <c r="G79" s="5" t="s">
+      <c r="G79" s="4" t="s">
         <v>302</v>
       </c>
     </row>
@@ -4982,9 +4979,9 @@
       <c r="C80" t="s">
         <v>305</v>
       </c>
-      <c r="E80" s="5"/>
-      <c r="F80" s="5"/>
-      <c r="G80" s="5"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4"/>
+      <c r="G80" s="4"/>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" t="s">
@@ -4996,13 +4993,13 @@
       <c r="C81" t="s">
         <v>308</v>
       </c>
-      <c r="E81" s="5" t="s">
+      <c r="E81" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F81" s="5">
+      <c r="F81" s="4">
         <v>8646</v>
       </c>
-      <c r="G81" s="5" t="s">
+      <c r="G81" s="4" t="s">
         <v>308</v>
       </c>
     </row>
@@ -5016,9 +5013,9 @@
       <c r="C82" t="s">
         <v>311</v>
       </c>
-      <c r="E82" s="5"/>
-      <c r="F82" s="5"/>
-      <c r="G82" s="5"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="4"/>
+      <c r="G82" s="4"/>
     </row>
     <row r="83" spans="1:7">
       <c r="A83" t="s">
@@ -5030,9 +5027,9 @@
       <c r="C83" t="s">
         <v>314</v>
       </c>
-      <c r="E83" s="5"/>
-      <c r="F83" s="5"/>
-      <c r="G83" s="5"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="4"/>
+      <c r="G83" s="4"/>
     </row>
     <row r="84" spans="1:7">
       <c r="A84" t="s">
@@ -5044,9 +5041,9 @@
       <c r="C84" t="s">
         <v>317</v>
       </c>
-      <c r="E84" s="5"/>
-      <c r="F84" s="5"/>
-      <c r="G84" s="5"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="4"/>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" t="s">
@@ -5058,13 +5055,13 @@
       <c r="C85" t="s">
         <v>320</v>
       </c>
-      <c r="E85" s="5" t="s">
+      <c r="E85" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F85" s="5">
+      <c r="F85" s="4">
         <v>28</v>
       </c>
-      <c r="G85" s="5" t="s">
+      <c r="G85" s="4" t="s">
         <v>320</v>
       </c>
     </row>
@@ -5078,9 +5075,9 @@
       <c r="C86" t="s">
         <v>323</v>
       </c>
-      <c r="E86" s="5"/>
-      <c r="F86" s="5"/>
-      <c r="G86" s="5"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="4"/>
+      <c r="G86" s="4"/>
     </row>
     <row r="87" spans="1:7">
       <c r="A87" t="s">
@@ -5092,9 +5089,9 @@
       <c r="C87" t="s">
         <v>326</v>
       </c>
-      <c r="E87" s="5"/>
-      <c r="F87" s="5"/>
-      <c r="G87" s="5"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="4"/>
+      <c r="G87" s="4"/>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" t="s">
@@ -5106,9 +5103,9 @@
       <c r="C88" t="s">
         <v>329</v>
       </c>
-      <c r="E88" s="5"/>
-      <c r="F88" s="5"/>
-      <c r="G88" s="5"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="4"/>
     </row>
     <row r="89" spans="1:7">
       <c r="A89" t="s">
@@ -5120,13 +5117,13 @@
       <c r="C89" t="s">
         <v>332</v>
       </c>
-      <c r="E89" s="5" t="s">
+      <c r="E89" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F89" s="5">
+      <c r="F89" s="4">
         <v>9676</v>
       </c>
-      <c r="G89" s="5" t="s">
+      <c r="G89" s="4" t="s">
         <v>332</v>
       </c>
     </row>
@@ -5140,9 +5137,9 @@
       <c r="C90" t="s">
         <v>335</v>
       </c>
-      <c r="E90" s="5"/>
-      <c r="F90" s="5"/>
-      <c r="G90" s="5"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="4"/>
     </row>
     <row r="91" spans="1:7">
       <c r="A91" t="s">
@@ -5154,9 +5151,9 @@
       <c r="C91" t="s">
         <v>338</v>
       </c>
-      <c r="E91" s="5"/>
-      <c r="F91" s="5"/>
-      <c r="G91" s="5"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="4"/>
+      <c r="G91" s="4"/>
     </row>
     <row r="92" spans="1:7">
       <c r="A92" t="s">
@@ -5168,9 +5165,9 @@
       <c r="C92" t="s">
         <v>341</v>
       </c>
-      <c r="E92" s="5"/>
-      <c r="F92" s="5"/>
-      <c r="G92" s="5"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="4"/>
+      <c r="G92" s="4"/>
     </row>
     <row r="93" spans="1:7">
       <c r="A93" t="s">
@@ -5182,9 +5179,9 @@
       <c r="C93" t="s">
         <v>344</v>
       </c>
-      <c r="E93" s="5"/>
-      <c r="F93" s="5"/>
-      <c r="G93" s="5"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="4"/>
+      <c r="G93" s="4"/>
     </row>
     <row r="94" spans="1:7">
       <c r="A94" t="s">
@@ -5196,9 +5193,9 @@
       <c r="C94" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="E94" s="5"/>
-      <c r="F94" s="5"/>
-      <c r="G94" s="5"/>
+      <c r="E94" s="4"/>
+      <c r="F94" s="4"/>
+      <c r="G94" s="4"/>
     </row>
     <row r="95" spans="1:7">
       <c r="A95" t="s">
@@ -5210,13 +5207,13 @@
       <c r="C95" t="s">
         <v>350</v>
       </c>
-      <c r="E95" s="5" t="s">
+      <c r="E95" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F95" s="5">
+      <c r="F95" s="4">
         <v>785</v>
       </c>
-      <c r="G95" s="5" t="s">
+      <c r="G95" s="4" t="s">
         <v>350</v>
       </c>
     </row>
@@ -5230,13 +5227,13 @@
       <c r="C96" t="s">
         <v>353</v>
       </c>
-      <c r="E96" s="5" t="s">
+      <c r="E96" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F96" s="5">
+      <c r="F96" s="4">
         <v>766</v>
       </c>
-      <c r="G96" s="5" t="s">
+      <c r="G96" s="4" t="s">
         <v>353</v>
       </c>
     </row>
@@ -5250,9 +5247,9 @@
       <c r="C97" t="s">
         <v>356</v>
       </c>
-      <c r="E97" s="5"/>
-      <c r="F97" s="5"/>
-      <c r="G97" s="5"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="4"/>
+      <c r="G97" s="4"/>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" t="s">
@@ -5264,9 +5261,9 @@
       <c r="C98" t="s">
         <v>359</v>
       </c>
-      <c r="E98" s="5"/>
-      <c r="F98" s="5"/>
-      <c r="G98" s="5"/>
+      <c r="E98" s="4"/>
+      <c r="F98" s="4"/>
+      <c r="G98" s="4"/>
     </row>
     <row r="99" spans="1:7">
       <c r="A99" t="s">
@@ -5278,9 +5275,9 @@
       <c r="C99" t="s">
         <v>362</v>
       </c>
-      <c r="E99" s="5"/>
-      <c r="F99" s="5"/>
-      <c r="G99" s="5"/>
+      <c r="E99" s="4"/>
+      <c r="F99" s="4"/>
+      <c r="G99" s="4"/>
     </row>
     <row r="100" spans="1:7">
       <c r="A100" t="s">
@@ -5292,9 +5289,9 @@
       <c r="C100" t="s">
         <v>365</v>
       </c>
-      <c r="E100" s="5"/>
-      <c r="F100" s="5"/>
-      <c r="G100" s="5"/>
+      <c r="E100" s="4"/>
+      <c r="F100" s="4"/>
+      <c r="G100" s="4"/>
     </row>
     <row r="101" spans="1:7">
       <c r="A101" t="s">
@@ -5306,9 +5303,9 @@
       <c r="C101" t="s">
         <v>368</v>
       </c>
-      <c r="E101" s="5"/>
-      <c r="F101" s="5"/>
-      <c r="G101" s="5"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="4"/>
+      <c r="G101" s="4"/>
     </row>
     <row r="102" spans="1:7">
       <c r="A102" t="s">
@@ -5320,9 +5317,9 @@
       <c r="C102" t="s">
         <v>371</v>
       </c>
-      <c r="E102" s="5"/>
-      <c r="F102" s="5"/>
-      <c r="G102" s="5"/>
+      <c r="E102" s="4"/>
+      <c r="F102" s="4"/>
+      <c r="G102" s="4"/>
     </row>
     <row r="103" spans="1:7">
       <c r="A103" t="s">
@@ -5334,9 +5331,9 @@
       <c r="C103" t="s">
         <v>374</v>
       </c>
-      <c r="E103" s="5"/>
-      <c r="F103" s="5"/>
-      <c r="G103" s="5"/>
+      <c r="E103" s="4"/>
+      <c r="F103" s="4"/>
+      <c r="G103" s="4"/>
     </row>
     <row r="104" spans="1:7">
       <c r="A104" t="s">
@@ -5348,9 +5345,9 @@
       <c r="C104" t="s">
         <v>377</v>
       </c>
-      <c r="E104" s="5"/>
-      <c r="F104" s="5"/>
-      <c r="G104" s="5"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="4"/>
+      <c r="G104" s="4"/>
     </row>
     <row r="105" spans="1:7">
       <c r="A105" t="s">
@@ -5362,13 +5359,13 @@
       <c r="C105" t="s">
         <v>380</v>
       </c>
-      <c r="E105" s="5" t="s">
+      <c r="E105" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F105" s="5">
+      <c r="F105" s="4">
         <v>5785</v>
       </c>
-      <c r="G105" s="5" t="s">
+      <c r="G105" s="4" t="s">
         <v>380</v>
       </c>
     </row>
@@ -5382,9 +5379,9 @@
       <c r="C106" t="s">
         <v>383</v>
       </c>
-      <c r="E106" s="5"/>
-      <c r="F106" s="5"/>
-      <c r="G106" s="5"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="4"/>
+      <c r="G106" s="4"/>
     </row>
     <row r="107" spans="1:7">
       <c r="A107" t="s">
@@ -5396,9 +5393,9 @@
       <c r="C107" t="s">
         <v>386</v>
       </c>
-      <c r="E107" s="5"/>
-      <c r="F107" s="5"/>
-      <c r="G107" s="5"/>
+      <c r="E107" s="4"/>
+      <c r="F107" s="4"/>
+      <c r="G107" s="4"/>
     </row>
     <row r="108" spans="1:7">
       <c r="A108" t="s">
@@ -5410,9 +5407,9 @@
       <c r="C108" t="s">
         <v>389</v>
       </c>
-      <c r="E108" s="5"/>
-      <c r="F108" s="5"/>
-      <c r="G108" s="5"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="4"/>
+      <c r="G108" s="4"/>
     </row>
     <row r="109" spans="1:7">
       <c r="A109" t="s">
@@ -5424,9 +5421,9 @@
       <c r="C109" t="s">
         <v>392</v>
       </c>
-      <c r="E109" s="5"/>
-      <c r="F109" s="5"/>
-      <c r="G109" s="5"/>
+      <c r="E109" s="4"/>
+      <c r="F109" s="4"/>
+      <c r="G109" s="4"/>
     </row>
     <row r="110" spans="1:7">
       <c r="A110" t="s">
@@ -5438,13 +5435,13 @@
       <c r="C110" t="s">
         <v>395</v>
       </c>
-      <c r="E110" s="5" t="s">
+      <c r="E110" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F110" s="5">
+      <c r="F110" s="4">
         <v>347</v>
       </c>
-      <c r="G110" s="5" t="s">
+      <c r="G110" s="4" t="s">
         <v>395</v>
       </c>
     </row>
@@ -5458,13 +5455,13 @@
       <c r="C111" t="s">
         <v>398</v>
       </c>
-      <c r="E111" s="5" t="s">
+      <c r="E111" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F111" s="5">
+      <c r="F111" s="4">
         <v>854</v>
       </c>
-      <c r="G111" s="5" t="s">
+      <c r="G111" s="4" t="s">
         <v>398</v>
       </c>
     </row>
@@ -5478,9 +5475,9 @@
       <c r="C112" t="s">
         <v>401</v>
       </c>
-      <c r="E112" s="5"/>
-      <c r="F112" s="5"/>
-      <c r="G112" s="5"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="4"/>
+      <c r="G112" s="4"/>
     </row>
     <row r="113" spans="1:7">
       <c r="A113" t="s">
@@ -5492,9 +5489,9 @@
       <c r="C113" t="s">
         <v>404</v>
       </c>
-      <c r="E113" s="5"/>
-      <c r="F113" s="5"/>
-      <c r="G113" s="5"/>
+      <c r="E113" s="4"/>
+      <c r="F113" s="4"/>
+      <c r="G113" s="4"/>
     </row>
     <row r="114" spans="1:7">
       <c r="A114" t="s">
@@ -5506,9 +5503,9 @@
       <c r="C114" t="s">
         <v>407</v>
       </c>
-      <c r="E114" s="5"/>
-      <c r="F114" s="5"/>
-      <c r="G114" s="5"/>
+      <c r="E114" s="4"/>
+      <c r="F114" s="4"/>
+      <c r="G114" s="4"/>
     </row>
     <row r="115" spans="1:7">
       <c r="A115" t="s">
@@ -5520,13 +5517,13 @@
       <c r="C115" t="s">
         <v>410</v>
       </c>
-      <c r="E115" s="5" t="s">
+      <c r="E115" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F115" s="5">
+      <c r="F115" s="4">
         <v>211</v>
       </c>
-      <c r="G115" s="5" t="s">
+      <c r="G115" s="4" t="s">
         <v>410</v>
       </c>
     </row>
@@ -5540,9 +5537,9 @@
       <c r="C116" t="s">
         <v>413</v>
       </c>
-      <c r="E116" s="5"/>
-      <c r="F116" s="5"/>
-      <c r="G116" s="5"/>
+      <c r="E116" s="4"/>
+      <c r="F116" s="4"/>
+      <c r="G116" s="4"/>
     </row>
     <row r="117" spans="1:7">
       <c r="A117" t="s">
@@ -5554,9 +5551,9 @@
       <c r="C117" t="s">
         <v>416</v>
       </c>
-      <c r="E117" s="5"/>
-      <c r="F117" s="5"/>
-      <c r="G117" s="5"/>
+      <c r="E117" s="4"/>
+      <c r="F117" s="4"/>
+      <c r="G117" s="4"/>
     </row>
     <row r="118" spans="1:7">
       <c r="A118" t="s">
@@ -5568,9 +5565,9 @@
       <c r="C118" t="s">
         <v>419</v>
       </c>
-      <c r="E118" s="5"/>
-      <c r="F118" s="5"/>
-      <c r="G118" s="5"/>
+      <c r="E118" s="4"/>
+      <c r="F118" s="4"/>
+      <c r="G118" s="4"/>
     </row>
     <row r="119" spans="1:7">
       <c r="A119" t="s">
@@ -5582,9 +5579,9 @@
       <c r="C119" t="s">
         <v>422</v>
       </c>
-      <c r="E119" s="5"/>
-      <c r="F119" s="5"/>
-      <c r="G119" s="5"/>
+      <c r="E119" s="4"/>
+      <c r="F119" s="4"/>
+      <c r="G119" s="4"/>
     </row>
     <row r="120" spans="1:7">
       <c r="A120" t="s">
@@ -5596,9 +5593,9 @@
       <c r="C120" t="s">
         <v>425</v>
       </c>
-      <c r="E120" s="5"/>
-      <c r="F120" s="5"/>
-      <c r="G120" s="5"/>
+      <c r="E120" s="4"/>
+      <c r="F120" s="4"/>
+      <c r="G120" s="4"/>
     </row>
     <row r="121" spans="1:7">
       <c r="A121" t="s">
@@ -5610,9 +5607,9 @@
       <c r="C121" t="s">
         <v>428</v>
       </c>
-      <c r="E121" s="5"/>
-      <c r="F121" s="5"/>
-      <c r="G121" s="5"/>
+      <c r="E121" s="4"/>
+      <c r="F121" s="4"/>
+      <c r="G121" s="4"/>
     </row>
     <row r="122" spans="1:7">
       <c r="A122" t="s">
@@ -5624,9 +5621,9 @@
       <c r="C122" t="s">
         <v>431</v>
       </c>
-      <c r="E122" s="5"/>
-      <c r="F122" s="5"/>
-      <c r="G122" s="5"/>
+      <c r="E122" s="4"/>
+      <c r="F122" s="4"/>
+      <c r="G122" s="4"/>
     </row>
     <row r="123" spans="1:7">
       <c r="A123" t="s">
@@ -5638,9 +5635,9 @@
       <c r="C123" t="s">
         <v>434</v>
       </c>
-      <c r="E123" s="5"/>
-      <c r="F123" s="5"/>
-      <c r="G123" s="5"/>
+      <c r="E123" s="4"/>
+      <c r="F123" s="4"/>
+      <c r="G123" s="4"/>
     </row>
     <row r="124" spans="1:7">
       <c r="A124" t="s">
@@ -5652,9 +5649,9 @@
       <c r="C124" t="s">
         <v>437</v>
       </c>
-      <c r="E124" s="5"/>
-      <c r="F124" s="5"/>
-      <c r="G124" s="5"/>
+      <c r="E124" s="4"/>
+      <c r="F124" s="4"/>
+      <c r="G124" s="4"/>
     </row>
     <row r="125" spans="1:7">
       <c r="A125" t="s">
@@ -5666,9 +5663,9 @@
       <c r="C125" t="s">
         <v>440</v>
       </c>
-      <c r="E125" s="5"/>
-      <c r="F125" s="5"/>
-      <c r="G125" s="5"/>
+      <c r="E125" s="4"/>
+      <c r="F125" s="4"/>
+      <c r="G125" s="4"/>
     </row>
     <row r="126" spans="1:7">
       <c r="A126" t="s">
@@ -5680,13 +5677,13 @@
       <c r="C126" t="s">
         <v>443</v>
       </c>
-      <c r="E126" s="5" t="s">
+      <c r="E126" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F126" s="5">
+      <c r="F126" s="4">
         <v>711</v>
       </c>
-      <c r="G126" s="5" t="s">
+      <c r="G126" s="4" t="s">
         <v>443</v>
       </c>
     </row>
@@ -5700,13 +5697,13 @@
       <c r="C127" t="s">
         <v>446</v>
       </c>
-      <c r="E127" s="5" t="s">
+      <c r="E127" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F127" s="5">
+      <c r="F127" s="4">
         <v>14773</v>
       </c>
-      <c r="G127" s="5" t="s">
+      <c r="G127" s="4" t="s">
         <v>446</v>
       </c>
     </row>
@@ -5720,13 +5717,13 @@
       <c r="C128" t="s">
         <v>449</v>
       </c>
-      <c r="E128" s="5" t="s">
+      <c r="E128" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F128" s="5">
+      <c r="F128" s="4">
         <v>17054</v>
       </c>
-      <c r="G128" s="5" t="s">
+      <c r="G128" s="4" t="s">
         <v>449</v>
       </c>
     </row>
@@ -5740,13 +5737,13 @@
       <c r="C129" t="s">
         <v>452</v>
       </c>
-      <c r="E129" s="5" t="s">
+      <c r="E129" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F129" s="5">
+      <c r="F129" s="4">
         <v>233</v>
       </c>
-      <c r="G129" s="5" t="s">
+      <c r="G129" s="4" t="s">
         <v>452</v>
       </c>
     </row>
@@ -5760,9 +5757,9 @@
       <c r="C130" t="s">
         <v>455</v>
       </c>
-      <c r="E130" s="5"/>
-      <c r="F130" s="5"/>
-      <c r="G130" s="5"/>
+      <c r="E130" s="4"/>
+      <c r="F130" s="4"/>
+      <c r="G130" s="4"/>
     </row>
     <row r="131" spans="1:7">
       <c r="A131" t="s">
@@ -5774,13 +5771,13 @@
       <c r="C131" t="s">
         <v>458</v>
       </c>
-      <c r="E131" s="5" t="s">
+      <c r="E131" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F131" s="5">
+      <c r="F131" s="4">
         <v>826</v>
       </c>
-      <c r="G131" s="5" t="s">
+      <c r="G131" s="4" t="s">
         <v>458</v>
       </c>
     </row>
@@ -5794,9 +5791,9 @@
       <c r="C132" t="s">
         <v>461</v>
       </c>
-      <c r="E132" s="5"/>
-      <c r="F132" s="5"/>
-      <c r="G132" s="5"/>
+      <c r="E132" s="4"/>
+      <c r="F132" s="4"/>
+      <c r="G132" s="4"/>
     </row>
     <row r="133" spans="1:7">
       <c r="A133" t="s">
@@ -5808,9 +5805,9 @@
       <c r="C133" t="s">
         <v>464</v>
       </c>
-      <c r="E133" s="5"/>
-      <c r="F133" s="5"/>
-      <c r="G133" s="5"/>
+      <c r="E133" s="4"/>
+      <c r="F133" s="4"/>
+      <c r="G133" s="4"/>
     </row>
     <row r="134" spans="1:7">
       <c r="A134" t="s">
@@ -5822,9 +5819,9 @@
       <c r="C134" t="s">
         <v>467</v>
       </c>
-      <c r="E134" s="5"/>
-      <c r="F134" s="5"/>
-      <c r="G134" s="5"/>
+      <c r="E134" s="4"/>
+      <c r="F134" s="4"/>
+      <c r="G134" s="4"/>
     </row>
     <row r="135" spans="1:7">
       <c r="A135" t="s">
@@ -5836,9 +5833,9 @@
       <c r="C135" t="s">
         <v>470</v>
       </c>
-      <c r="E135" s="5"/>
-      <c r="F135" s="5"/>
-      <c r="G135" s="5"/>
+      <c r="E135" s="4"/>
+      <c r="F135" s="4"/>
+      <c r="G135" s="4"/>
     </row>
     <row r="136" spans="1:7">
       <c r="A136" t="s">
@@ -5850,9 +5847,9 @@
       <c r="C136" t="s">
         <v>473</v>
       </c>
-      <c r="E136" s="5"/>
-      <c r="F136" s="5"/>
-      <c r="G136" s="5"/>
+      <c r="E136" s="4"/>
+      <c r="F136" s="4"/>
+      <c r="G136" s="4"/>
     </row>
     <row r="137" spans="1:7">
       <c r="A137" t="s">
@@ -5864,13 +5861,13 @@
       <c r="C137" t="s">
         <v>476</v>
       </c>
-      <c r="E137" s="5" t="s">
+      <c r="E137" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F137" s="5">
+      <c r="F137" s="4">
         <v>33788</v>
       </c>
-      <c r="G137" s="5" t="s">
+      <c r="G137" s="4" t="s">
         <v>476</v>
       </c>
     </row>
@@ -5884,9 +5881,9 @@
       <c r="C138" t="s">
         <v>479</v>
       </c>
-      <c r="E138" s="5"/>
-      <c r="F138" s="5"/>
-      <c r="G138" s="5"/>
+      <c r="E138" s="4"/>
+      <c r="F138" s="4"/>
+      <c r="G138" s="4"/>
     </row>
     <row r="139" spans="1:7">
       <c r="A139" t="s">
@@ -5898,9 +5895,9 @@
       <c r="C139" t="s">
         <v>482</v>
       </c>
-      <c r="E139" s="5"/>
-      <c r="F139" s="5"/>
-      <c r="G139" s="5"/>
+      <c r="E139" s="4"/>
+      <c r="F139" s="4"/>
+      <c r="G139" s="4"/>
     </row>
     <row r="140" spans="1:7">
       <c r="A140" t="s">
@@ -5912,9 +5909,9 @@
       <c r="C140" t="s">
         <v>485</v>
       </c>
-      <c r="E140" s="5"/>
-      <c r="F140" s="5"/>
-      <c r="G140" s="5"/>
+      <c r="E140" s="4"/>
+      <c r="F140" s="4"/>
+      <c r="G140" s="4"/>
     </row>
     <row r="141" spans="1:7">
       <c r="A141" t="s">
@@ -5926,9 +5923,9 @@
       <c r="C141" t="s">
         <v>488</v>
       </c>
-      <c r="E141" s="5"/>
-      <c r="F141" s="5"/>
-      <c r="G141" s="5"/>
+      <c r="E141" s="4"/>
+      <c r="F141" s="4"/>
+      <c r="G141" s="4"/>
     </row>
     <row r="142" spans="1:7">
       <c r="A142" t="s">
@@ -5940,9 +5937,9 @@
       <c r="C142" t="s">
         <v>491</v>
       </c>
-      <c r="E142" s="5"/>
-      <c r="F142" s="5"/>
-      <c r="G142" s="5"/>
+      <c r="E142" s="4"/>
+      <c r="F142" s="4"/>
+      <c r="G142" s="4"/>
     </row>
     <row r="143" spans="1:7">
       <c r="A143" t="s">
@@ -5954,9 +5951,9 @@
       <c r="C143" t="s">
         <v>494</v>
       </c>
-      <c r="E143" s="5"/>
-      <c r="F143" s="5"/>
-      <c r="G143" s="5"/>
+      <c r="E143" s="4"/>
+      <c r="F143" s="4"/>
+      <c r="G143" s="4"/>
     </row>
     <row r="144" spans="1:7">
       <c r="A144" t="s">
@@ -5968,9 +5965,9 @@
       <c r="C144" t="s">
         <v>497</v>
       </c>
-      <c r="E144" s="5"/>
-      <c r="F144" s="5"/>
-      <c r="G144" s="5"/>
+      <c r="E144" s="4"/>
+      <c r="F144" s="4"/>
+      <c r="G144" s="4"/>
     </row>
     <row r="145" spans="1:7">
       <c r="A145" t="s">
@@ -5982,9 +5979,9 @@
       <c r="C145" t="s">
         <v>500</v>
       </c>
-      <c r="E145" s="5"/>
-      <c r="F145" s="5"/>
-      <c r="G145" s="5"/>
+      <c r="E145" s="4"/>
+      <c r="F145" s="4"/>
+      <c r="G145" s="4"/>
     </row>
     <row r="146" spans="1:7">
       <c r="A146" t="s">
@@ -5996,13 +5993,13 @@
       <c r="C146" t="s">
         <v>503</v>
       </c>
-      <c r="E146" s="5" t="s">
+      <c r="E146" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F146" s="5">
+      <c r="F146" s="4">
         <v>30971</v>
       </c>
-      <c r="G146" s="5" t="s">
+      <c r="G146" s="4" t="s">
         <v>503</v>
       </c>
     </row>
@@ -6016,9 +6013,9 @@
       <c r="C147" t="s">
         <v>506</v>
       </c>
-      <c r="E147" s="5"/>
-      <c r="F147" s="5"/>
-      <c r="G147" s="5"/>
+      <c r="E147" s="4"/>
+      <c r="F147" s="4"/>
+      <c r="G147" s="4"/>
     </row>
     <row r="148" spans="1:7">
       <c r="A148" t="s">
@@ -6030,13 +6027,13 @@
       <c r="C148" t="s">
         <v>509</v>
       </c>
-      <c r="E148" s="5" t="s">
+      <c r="E148" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F148" s="5">
+      <c r="F148" s="4">
         <v>928</v>
       </c>
-      <c r="G148" s="5" t="s">
+      <c r="G148" s="4" t="s">
         <v>509</v>
       </c>
     </row>
@@ -6050,9 +6047,9 @@
       <c r="C149" t="s">
         <v>512</v>
       </c>
-      <c r="E149" s="5"/>
-      <c r="F149" s="5"/>
-      <c r="G149" s="5"/>
+      <c r="E149" s="4"/>
+      <c r="F149" s="4"/>
+      <c r="G149" s="4"/>
     </row>
     <row r="150" spans="1:7">
       <c r="A150" t="s">
@@ -6064,9 +6061,9 @@
       <c r="C150" t="s">
         <v>515</v>
       </c>
-      <c r="E150" s="5"/>
-      <c r="F150" s="5"/>
-      <c r="G150" s="5"/>
+      <c r="E150" s="4"/>
+      <c r="F150" s="4"/>
+      <c r="G150" s="4"/>
     </row>
     <row r="151" spans="1:7">
       <c r="A151" t="s">
@@ -6081,13 +6078,13 @@
       <c r="D151" t="s">
         <v>57</v>
       </c>
-      <c r="E151" s="5" t="s">
+      <c r="E151" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F151" s="5">
+      <c r="F151" s="4">
         <v>1183</v>
       </c>
-      <c r="G151" s="5" t="s">
+      <c r="G151" s="4" t="s">
         <v>518</v>
       </c>
     </row>
@@ -6101,13 +6098,13 @@
       <c r="C152" t="s">
         <v>521</v>
       </c>
-      <c r="E152" s="5" t="s">
+      <c r="E152" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F152" s="5">
+      <c r="F152" s="4">
         <v>407199</v>
       </c>
-      <c r="G152" s="5" t="s">
+      <c r="G152" s="4" t="s">
         <v>521</v>
       </c>
     </row>
@@ -6121,9 +6118,9 @@
       <c r="C153" t="s">
         <v>524</v>
       </c>
-      <c r="E153" s="5"/>
-      <c r="F153" s="5"/>
-      <c r="G153" s="5"/>
+      <c r="E153" s="4"/>
+      <c r="F153" s="4"/>
+      <c r="G153" s="4"/>
     </row>
     <row r="154" spans="1:7">
       <c r="A154" t="s">
@@ -6135,9 +6132,9 @@
       <c r="C154" t="s">
         <v>527</v>
       </c>
-      <c r="E154" s="5"/>
-      <c r="F154" s="5"/>
-      <c r="G154" s="5"/>
+      <c r="E154" s="4"/>
+      <c r="F154" s="4"/>
+      <c r="G154" s="4"/>
     </row>
     <row r="155" spans="1:7">
       <c r="A155" t="s">
@@ -6149,9 +6146,9 @@
       <c r="C155" t="s">
         <v>530</v>
       </c>
-      <c r="E155" s="5"/>
-      <c r="F155" s="5"/>
-      <c r="G155" s="5"/>
+      <c r="E155" s="4"/>
+      <c r="F155" s="4"/>
+      <c r="G155" s="4"/>
     </row>
     <row r="156" spans="1:7">
       <c r="A156" t="s">
@@ -6163,13 +6160,13 @@
       <c r="C156" t="s">
         <v>533</v>
       </c>
-      <c r="E156" s="5" t="s">
+      <c r="E156" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F156" s="5">
+      <c r="F156" s="4">
         <v>17070</v>
       </c>
-      <c r="G156" s="5" t="s">
+      <c r="G156" s="4" t="s">
         <v>533</v>
       </c>
     </row>
@@ -6183,9 +6180,9 @@
       <c r="C157" t="s">
         <v>536</v>
       </c>
-      <c r="E157" s="5"/>
-      <c r="F157" s="5"/>
-      <c r="G157" s="5"/>
+      <c r="E157" s="4"/>
+      <c r="F157" s="4"/>
+      <c r="G157" s="4"/>
     </row>
     <row r="158" spans="1:7">
       <c r="A158" t="s">
@@ -6197,13 +6194,13 @@
       <c r="C158" t="s">
         <v>539</v>
       </c>
-      <c r="E158" s="5" t="s">
+      <c r="E158" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F158" s="5">
+      <c r="F158" s="4">
         <v>403</v>
       </c>
-      <c r="G158" s="5" t="s">
+      <c r="G158" s="4" t="s">
         <v>539</v>
       </c>
     </row>
@@ -6217,13 +6214,13 @@
       <c r="C159" t="s">
         <v>542</v>
       </c>
-      <c r="E159" s="5" t="s">
+      <c r="E159" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F159" s="5">
+      <c r="F159" s="4">
         <v>159</v>
       </c>
-      <c r="G159" s="5" t="s">
+      <c r="G159" s="4" t="s">
         <v>542</v>
       </c>
     </row>
@@ -6237,9 +6234,9 @@
       <c r="C160" t="s">
         <v>545</v>
       </c>
-      <c r="E160" s="5"/>
-      <c r="F160" s="5"/>
-      <c r="G160" s="5"/>
+      <c r="E160" s="4"/>
+      <c r="F160" s="4"/>
+      <c r="G160" s="4"/>
     </row>
     <row r="161" spans="1:7">
       <c r="A161" t="s">
@@ -6251,9 +6248,9 @@
       <c r="C161" t="s">
         <v>548</v>
       </c>
-      <c r="E161" s="5"/>
-      <c r="F161" s="5"/>
-      <c r="G161" s="5"/>
+      <c r="E161" s="4"/>
+      <c r="F161" s="4"/>
+      <c r="G161" s="4"/>
     </row>
     <row r="162" spans="1:7">
       <c r="A162" t="s">
@@ -6265,9 +6262,9 @@
       <c r="C162" t="s">
         <v>551</v>
       </c>
-      <c r="E162" s="5"/>
-      <c r="F162" s="5"/>
-      <c r="G162" s="5"/>
+      <c r="E162" s="4"/>
+      <c r="F162" s="4"/>
+      <c r="G162" s="4"/>
     </row>
     <row r="163" spans="1:7">
       <c r="A163" t="s">
@@ -6279,9 +6276,9 @@
       <c r="C163" t="s">
         <v>554</v>
       </c>
-      <c r="E163" s="5"/>
-      <c r="F163" s="5"/>
-      <c r="G163" s="5"/>
+      <c r="E163" s="4"/>
+      <c r="F163" s="4"/>
+      <c r="G163" s="4"/>
     </row>
     <row r="164" spans="1:7">
       <c r="A164" t="s">
@@ -6293,9 +6290,9 @@
       <c r="C164" t="s">
         <v>557</v>
       </c>
-      <c r="E164" s="5"/>
-      <c r="F164" s="5"/>
-      <c r="G164" s="5"/>
+      <c r="E164" s="4"/>
+      <c r="F164" s="4"/>
+      <c r="G164" s="4"/>
     </row>
     <row r="165" spans="1:7">
       <c r="A165" t="s">
@@ -6307,9 +6304,9 @@
       <c r="C165" t="s">
         <v>560</v>
       </c>
-      <c r="E165" s="5"/>
-      <c r="F165" s="5"/>
-      <c r="G165" s="5"/>
+      <c r="E165" s="4"/>
+      <c r="F165" s="4"/>
+      <c r="G165" s="4"/>
     </row>
     <row r="166" spans="1:7">
       <c r="A166" t="s">
@@ -6321,9 +6318,9 @@
       <c r="C166" t="s">
         <v>563</v>
       </c>
-      <c r="E166" s="5"/>
-      <c r="F166" s="5"/>
-      <c r="G166" s="5"/>
+      <c r="E166" s="4"/>
+      <c r="F166" s="4"/>
+      <c r="G166" s="4"/>
     </row>
     <row r="167" spans="1:7">
       <c r="A167" t="s">
@@ -6335,13 +6332,13 @@
       <c r="C167" t="s">
         <v>566</v>
       </c>
-      <c r="E167" s="5" t="s">
+      <c r="E167" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F167" s="5">
+      <c r="F167" s="4">
         <v>215</v>
       </c>
-      <c r="G167" s="5" t="s">
+      <c r="G167" s="4" t="s">
         <v>566</v>
       </c>
     </row>
@@ -6355,9 +6352,9 @@
       <c r="C168" t="s">
         <v>569</v>
       </c>
-      <c r="E168" s="5"/>
-      <c r="F168" s="5"/>
-      <c r="G168" s="5"/>
+      <c r="E168" s="4"/>
+      <c r="F168" s="4"/>
+      <c r="G168" s="4"/>
     </row>
     <row r="169" spans="1:7">
       <c r="A169" t="s">
@@ -6369,9 +6366,9 @@
       <c r="C169" t="s">
         <v>572</v>
       </c>
-      <c r="E169" s="5"/>
-      <c r="F169" s="5"/>
-      <c r="G169" s="5"/>
+      <c r="E169" s="4"/>
+      <c r="F169" s="4"/>
+      <c r="G169" s="4"/>
     </row>
     <row r="170" spans="1:7">
       <c r="A170" t="s">
@@ -6383,13 +6380,13 @@
       <c r="C170" t="s">
         <v>575</v>
       </c>
-      <c r="E170" s="5" t="s">
+      <c r="E170" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F170" s="5">
+      <c r="F170" s="4">
         <v>238</v>
       </c>
-      <c r="G170" s="5" t="s">
+      <c r="G170" s="4" t="s">
         <v>575</v>
       </c>
     </row>
@@ -6403,13 +6400,13 @@
       <c r="C171" t="s">
         <v>578</v>
       </c>
-      <c r="E171" s="5" t="s">
+      <c r="E171" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F171" s="5">
+      <c r="F171" s="4">
         <v>1041</v>
       </c>
-      <c r="G171" s="5" t="s">
+      <c r="G171" s="4" t="s">
         <v>578</v>
       </c>
     </row>
@@ -6423,9 +6420,9 @@
       <c r="C172" t="s">
         <v>581</v>
       </c>
-      <c r="E172" s="5"/>
-      <c r="F172" s="5"/>
-      <c r="G172" s="5"/>
+      <c r="E172" s="4"/>
+      <c r="F172" s="4"/>
+      <c r="G172" s="4"/>
     </row>
     <row r="173" spans="1:7">
       <c r="A173" t="s">
@@ -6437,9 +6434,9 @@
       <c r="C173" t="s">
         <v>584</v>
       </c>
-      <c r="E173" s="5"/>
-      <c r="F173" s="5"/>
-      <c r="G173" s="5"/>
+      <c r="E173" s="4"/>
+      <c r="F173" s="4"/>
+      <c r="G173" s="4"/>
     </row>
     <row r="174" spans="1:7">
       <c r="A174" t="s">
@@ -6451,13 +6448,13 @@
       <c r="C174" t="s">
         <v>587</v>
       </c>
-      <c r="E174" s="5" t="s">
+      <c r="E174" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F174" s="5">
+      <c r="F174" s="4">
         <v>958</v>
       </c>
-      <c r="G174" s="5" t="s">
+      <c r="G174" s="4" t="s">
         <v>587</v>
       </c>
     </row>
@@ -6471,9 +6468,9 @@
       <c r="C175" s="2" t="s">
         <v>590</v>
       </c>
-      <c r="E175" s="5"/>
-      <c r="F175" s="5"/>
-      <c r="G175" s="5"/>
+      <c r="E175" s="4"/>
+      <c r="F175" s="4"/>
+      <c r="G175" s="4"/>
     </row>
     <row r="176" spans="1:7">
       <c r="A176" t="s">
@@ -6485,9 +6482,9 @@
       <c r="C176" t="s">
         <v>593</v>
       </c>
-      <c r="E176" s="5"/>
-      <c r="F176" s="5"/>
-      <c r="G176" s="5"/>
+      <c r="E176" s="4"/>
+      <c r="F176" s="4"/>
+      <c r="G176" s="4"/>
     </row>
     <row r="177" spans="1:7">
       <c r="A177" t="s">
@@ -6499,13 +6496,13 @@
       <c r="C177" t="s">
         <v>596</v>
       </c>
-      <c r="E177" s="5" t="s">
+      <c r="E177" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F177" s="5">
+      <c r="F177" s="4">
         <v>858</v>
       </c>
-      <c r="G177" s="5" t="s">
+      <c r="G177" s="4" t="s">
         <v>596</v>
       </c>
     </row>
@@ -6519,9 +6516,9 @@
       <c r="C178" t="s">
         <v>599</v>
       </c>
-      <c r="E178" s="5"/>
-      <c r="F178" s="5"/>
-      <c r="G178" s="5"/>
+      <c r="E178" s="4"/>
+      <c r="F178" s="4"/>
+      <c r="G178" s="4"/>
     </row>
     <row r="179" spans="1:7">
       <c r="A179" t="s">
@@ -6533,9 +6530,9 @@
       <c r="C179" t="s">
         <v>602</v>
       </c>
-      <c r="E179" s="5"/>
-      <c r="F179" s="5"/>
-      <c r="G179" s="5"/>
+      <c r="E179" s="4"/>
+      <c r="F179" s="4"/>
+      <c r="G179" s="4"/>
     </row>
     <row r="180" spans="1:7">
       <c r="A180" t="s">
@@ -6547,9 +6544,9 @@
       <c r="C180" t="s">
         <v>605</v>
       </c>
-      <c r="E180" s="5"/>
-      <c r="F180" s="5"/>
-      <c r="G180" s="5"/>
+      <c r="E180" s="4"/>
+      <c r="F180" s="4"/>
+      <c r="G180" s="4"/>
     </row>
     <row r="181" spans="1:7">
       <c r="A181" t="s">
@@ -6561,13 +6558,13 @@
       <c r="C181" t="s">
         <v>608</v>
       </c>
-      <c r="E181" s="5" t="s">
+      <c r="E181" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F181" s="5">
+      <c r="F181" s="4">
         <v>863</v>
       </c>
-      <c r="G181" s="5" t="s">
+      <c r="G181" s="4" t="s">
         <v>608</v>
       </c>
     </row>
@@ -6581,9 +6578,9 @@
       <c r="C182" t="s">
         <v>611</v>
       </c>
-      <c r="E182" s="5"/>
-      <c r="F182" s="5"/>
-      <c r="G182" s="5"/>
+      <c r="E182" s="4"/>
+      <c r="F182" s="4"/>
+      <c r="G182" s="4"/>
     </row>
     <row r="183" spans="1:7">
       <c r="A183" t="s">
@@ -6595,9 +6592,9 @@
       <c r="C183" t="s">
         <v>614</v>
       </c>
-      <c r="E183" s="5"/>
-      <c r="F183" s="5"/>
-      <c r="G183" s="5"/>
+      <c r="E183" s="4"/>
+      <c r="F183" s="4"/>
+      <c r="G183" s="4"/>
     </row>
     <row r="184" spans="1:7">
       <c r="A184" t="s">
@@ -6609,9 +6606,9 @@
       <c r="C184" t="s">
         <v>617</v>
       </c>
-      <c r="E184" s="5"/>
-      <c r="F184" s="5"/>
-      <c r="G184" s="5"/>
+      <c r="E184" s="4"/>
+      <c r="F184" s="4"/>
+      <c r="G184" s="4"/>
     </row>
     <row r="185" spans="1:7">
       <c r="A185" t="s">
@@ -6623,13 +6620,13 @@
       <c r="C185" t="s">
         <v>620</v>
       </c>
-      <c r="E185" s="5" t="s">
+      <c r="E185" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F185" s="5">
+      <c r="F185" s="4">
         <v>754</v>
       </c>
-      <c r="G185" s="5" t="s">
+      <c r="G185" s="4" t="s">
         <v>620</v>
       </c>
     </row>
@@ -6643,9 +6640,9 @@
       <c r="C186" t="s">
         <v>623</v>
       </c>
-      <c r="E186" s="5"/>
-      <c r="F186" s="5"/>
-      <c r="G186" s="5"/>
+      <c r="E186" s="4"/>
+      <c r="F186" s="4"/>
+      <c r="G186" s="4"/>
     </row>
     <row r="187" spans="1:7">
       <c r="A187" t="s">
@@ -6657,9 +6654,9 @@
       <c r="C187" t="s">
         <v>626</v>
       </c>
-      <c r="E187" s="5"/>
-      <c r="F187" s="5"/>
-      <c r="G187" s="5"/>
+      <c r="E187" s="4"/>
+      <c r="F187" s="4"/>
+      <c r="G187" s="4"/>
     </row>
     <row r="188" spans="1:7">
       <c r="A188" t="s">
@@ -6671,9 +6668,9 @@
       <c r="C188" t="s">
         <v>629</v>
       </c>
-      <c r="E188" s="5"/>
-      <c r="F188" s="5"/>
-      <c r="G188" s="5"/>
+      <c r="E188" s="4"/>
+      <c r="F188" s="4"/>
+      <c r="G188" s="4"/>
     </row>
     <row r="189" spans="1:7">
       <c r="A189" t="s">
@@ -6685,9 +6682,9 @@
       <c r="C189" t="s">
         <v>632</v>
       </c>
-      <c r="E189" s="5"/>
-      <c r="F189" s="5"/>
-      <c r="G189" s="5"/>
+      <c r="E189" s="4"/>
+      <c r="F189" s="4"/>
+      <c r="G189" s="4"/>
     </row>
     <row r="190" spans="1:7">
       <c r="A190" t="s">
@@ -6699,9 +6696,9 @@
       <c r="C190" t="s">
         <v>635</v>
       </c>
-      <c r="E190" s="5"/>
-      <c r="F190" s="5"/>
-      <c r="G190" s="5"/>
+      <c r="E190" s="4"/>
+      <c r="F190" s="4"/>
+      <c r="G190" s="4"/>
     </row>
     <row r="191" spans="1:7">
       <c r="A191" t="s">
@@ -6713,9 +6710,9 @@
       <c r="C191" t="s">
         <v>638</v>
       </c>
-      <c r="E191" s="5"/>
-      <c r="F191" s="5"/>
-      <c r="G191" s="5"/>
+      <c r="E191" s="4"/>
+      <c r="F191" s="4"/>
+      <c r="G191" s="4"/>
     </row>
     <row r="192" spans="1:7">
       <c r="A192" t="s">
@@ -6727,9 +6724,9 @@
       <c r="C192" t="s">
         <v>641</v>
       </c>
-      <c r="E192" s="5"/>
-      <c r="F192" s="5"/>
-      <c r="G192" s="5"/>
+      <c r="E192" s="4"/>
+      <c r="F192" s="4"/>
+      <c r="G192" s="4"/>
     </row>
     <row r="193" spans="1:7">
       <c r="A193" t="s">
@@ -6741,9 +6738,9 @@
       <c r="C193" t="s">
         <v>644</v>
       </c>
-      <c r="E193" s="5"/>
-      <c r="F193" s="5"/>
-      <c r="G193" s="5"/>
+      <c r="E193" s="4"/>
+      <c r="F193" s="4"/>
+      <c r="G193" s="4"/>
     </row>
     <row r="194" spans="1:7">
       <c r="A194" t="s">
@@ -6755,9 +6752,9 @@
       <c r="C194" t="s">
         <v>647</v>
       </c>
-      <c r="E194" s="5"/>
-      <c r="F194" s="5"/>
-      <c r="G194" s="5"/>
+      <c r="E194" s="4"/>
+      <c r="F194" s="4"/>
+      <c r="G194" s="4"/>
     </row>
     <row r="195" spans="1:7">
       <c r="A195" t="s">
@@ -6769,9 +6766,9 @@
       <c r="C195" t="s">
         <v>650</v>
       </c>
-      <c r="E195" s="5"/>
-      <c r="F195" s="5"/>
-      <c r="G195" s="5"/>
+      <c r="E195" s="4"/>
+      <c r="F195" s="4"/>
+      <c r="G195" s="4"/>
     </row>
     <row r="196" spans="1:7">
       <c r="A196" t="s">
@@ -6783,13 +6780,13 @@
       <c r="C196" t="s">
         <v>653</v>
       </c>
-      <c r="E196" s="5" t="s">
+      <c r="E196" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F196" s="5">
+      <c r="F196" s="4">
         <v>25305</v>
       </c>
-      <c r="G196" s="5" t="s">
+      <c r="G196" s="4" t="s">
         <v>653</v>
       </c>
     </row>
@@ -6806,13 +6803,13 @@
       <c r="D197" t="s">
         <v>57</v>
       </c>
-      <c r="E197" s="5" t="s">
+      <c r="E197" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F197" s="5">
+      <c r="F197" s="4">
         <v>55614051</v>
       </c>
-      <c r="G197" s="5" t="s">
+      <c r="G197" s="4" t="s">
         <v>656</v>
       </c>
     </row>
@@ -6826,9 +6823,9 @@
       <c r="C198" t="s">
         <v>659</v>
       </c>
-      <c r="E198" s="5"/>
-      <c r="F198" s="5"/>
-      <c r="G198" s="5"/>
+      <c r="E198" s="4"/>
+      <c r="F198" s="4"/>
+      <c r="G198" s="4"/>
     </row>
     <row r="199" spans="1:7">
       <c r="A199" t="s">
@@ -6840,13 +6837,13 @@
       <c r="C199" t="s">
         <v>662</v>
       </c>
-      <c r="E199" s="5" t="s">
+      <c r="E199" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F199" s="5">
+      <c r="F199" s="4">
         <v>686</v>
       </c>
-      <c r="G199" s="5" t="s">
+      <c r="G199" s="4" t="s">
         <v>662</v>
       </c>
     </row>
@@ -6860,9 +6857,9 @@
       <c r="C200" t="s">
         <v>665</v>
       </c>
-      <c r="E200" s="5"/>
-      <c r="F200" s="5"/>
-      <c r="G200" s="5"/>
+      <c r="E200" s="4"/>
+      <c r="F200" s="4"/>
+      <c r="G200" s="4"/>
     </row>
     <row r="201" spans="1:7">
       <c r="A201" t="s">
@@ -6877,13 +6874,13 @@
       <c r="D201" t="s">
         <v>57</v>
       </c>
-      <c r="E201" s="5" t="s">
+      <c r="E201" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F201" s="5">
+      <c r="F201" s="4">
         <v>27778324</v>
       </c>
-      <c r="G201" s="5" t="s">
+      <c r="G201" s="4" t="s">
         <v>668</v>
       </c>
     </row>
@@ -6891,7 +6888,7 @@
       <c r="A202" t="s">
         <v>669</v>
       </c>
-      <c r="B202" s="6" t="s">
+      <c r="B202" s="5" t="s">
         <v>670</v>
       </c>
       <c r="C202" s="2" t="s">
@@ -7029,10 +7026,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -7043,7 +7040,7 @@
       <c r="A2" t="s">
         <v>692</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>693</v>
       </c>
     </row>
@@ -7075,7 +7072,7 @@
       <c r="A6" t="s">
         <v>700</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>701</v>
       </c>
     </row>
@@ -7178,10 +7175,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>716</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>717</v>
       </c>
     </row>
@@ -7229,13 +7226,13 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16.2734375" customWidth="1"/>
-    <col min="2" max="2" width="19.0078125" customWidth="1"/>
+    <col min="2" max="2" width="35.0234375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>